<commit_message>
Fix next.config.js eslintrc.json etc & Add Lint Format Storybook
</commit_message>
<xml_diff>
--- a/doc/20230202_ReactApp.xlsx
+++ b/doc/20230202_ReactApp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakip/Documents/theoriacode/jisyu/20230202_ReactApp/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1DD8A0D-B1E7-1C41-B7AD-2CACEE9C3277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08AE6692-F62D-2C42-BD5E-0D07D70F9DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="1500" windowWidth="28300" windowHeight="17440" activeTab="4" xr2:uid="{9D86ED21-1AC9-D642-9B74-F217DA55E7A3}"/>
+    <workbookView xWindow="2640" yWindow="1500" windowWidth="28300" windowHeight="17440" xr2:uid="{9D86ED21-1AC9-D642-9B74-F217DA55E7A3}"/>
   </bookViews>
   <sheets>
     <sheet name="予定成果物と開発環境" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>予定としている成果物</t>
     <rPh sb="0" eb="2">
@@ -300,13 +300,160 @@
   <si>
     <t>SSG + CSR のシーケンス図</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>▼ツール</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF2EAEBB"/>
+        <rFont val="Monaco"/>
+        <family val="2"/>
+      </rPr>
+      <t>react</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF2EAEBB"/>
+        <rFont val="Monaco"/>
+        <family val="2"/>
+      </rPr>
+      <t>react-dom</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF2EAEBB"/>
+        <rFont val="Monaco"/>
+        <family val="2"/>
+      </rPr>
+      <t>next</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF2EAEBB"/>
+        <rFont val="Monaco"/>
+        <family val="2"/>
+      </rPr>
+      <t>@next/font</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF2EAEBB"/>
+        <rFont val="Monaco"/>
+        <family val="2"/>
+      </rPr>
+      <t>typescript</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF2EAEBB"/>
+        <rFont val="Monaco"/>
+        <family val="2"/>
+      </rPr>
+      <t>@types/react</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF2EAEBB"/>
+        <rFont val="Monaco"/>
+        <family val="2"/>
+      </rPr>
+      <t>@types/node</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF2EAEBB"/>
+        <rFont val="Monaco"/>
+        <family val="2"/>
+      </rPr>
+      <t>@types/react-dom</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF2EAEBB"/>
+        <rFont val="Monaco"/>
+        <family val="2"/>
+      </rPr>
+      <t>eslint</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF2EAEBB"/>
+        <rFont val="Monaco"/>
+        <family val="2"/>
+      </rPr>
+      <t>eslint-config-next</t>
+    </r>
+  </si>
+  <si>
+    <t>npm install --save-dev prettier eslint typescript-eslint @typescript-eslint/eslint-plugin @typescript-eslint/parser eslint-config-prettier eslint-plugin-prettier eslint-plugin-react eslint-plugin-react-hooks eslint-plugin-import</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -331,8 +478,20 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2EAEBB"/>
+      <name val="Monaco"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFF2F2F2"/>
+      <name val="Monaco"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -348,6 +507,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -507,7 +672,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -575,6 +740,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1050,42 +1221,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A75F9DC-1CB6-7049-8E5D-3F652FE6EB52}">
-  <dimension ref="B2:J22"/>
+  <dimension ref="B2:AF22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
   <sheetData>
-    <row r="2" spans="2:10" ht="21" thickBot="1">
+    <row r="2" spans="2:32" ht="21" thickBot="1">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="2:10">
+    <row r="3" spans="2:32">
       <c r="C3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:10">
+    <row r="4" spans="2:32">
       <c r="C4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="21" thickBot="1">
+    <row r="6" spans="2:32" ht="21" thickBot="1">
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="2:10">
+    <row r="7" spans="2:32">
       <c r="C7" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="2:10">
+      <c r="M7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="2:32">
       <c r="D8" s="7" t="s">
         <v>4</v>
       </c>
@@ -1095,13 +1269,55 @@
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="6"/>
-    </row>
-    <row r="9" spans="2:10">
+      <c r="N8" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O8" s="24"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="24"/>
+      <c r="R8" s="24"/>
+      <c r="S8" s="24"/>
+      <c r="T8" s="24"/>
+      <c r="U8" s="24"/>
+      <c r="V8" s="24"/>
+      <c r="W8" s="24"/>
+      <c r="X8" s="24"/>
+      <c r="Y8" s="24"/>
+      <c r="Z8" s="24"/>
+      <c r="AA8" s="24"/>
+      <c r="AB8" s="24"/>
+      <c r="AC8" s="24"/>
+      <c r="AD8" s="24"/>
+      <c r="AE8" s="24"/>
+      <c r="AF8" s="24"/>
+    </row>
+    <row r="9" spans="2:32">
       <c r="C9" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="2:10">
+      <c r="N9" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="24"/>
+      <c r="R9" s="24"/>
+      <c r="S9" s="24"/>
+      <c r="T9" s="24"/>
+      <c r="U9" s="24"/>
+      <c r="V9" s="24"/>
+      <c r="W9" s="24"/>
+      <c r="X9" s="24"/>
+      <c r="Y9" s="24"/>
+      <c r="Z9" s="24"/>
+      <c r="AA9" s="24"/>
+      <c r="AB9" s="24"/>
+      <c r="AC9" s="24"/>
+      <c r="AD9" s="24"/>
+      <c r="AE9" s="24"/>
+      <c r="AF9" s="24"/>
+    </row>
+    <row r="10" spans="2:32">
       <c r="D10" s="7" t="s">
         <v>16</v>
       </c>
@@ -1111,13 +1327,55 @@
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="6"/>
-    </row>
-    <row r="11" spans="2:10">
+      <c r="N10" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="24"/>
+      <c r="S10" s="24"/>
+      <c r="T10" s="24"/>
+      <c r="U10" s="24"/>
+      <c r="V10" s="24"/>
+      <c r="W10" s="24"/>
+      <c r="X10" s="24"/>
+      <c r="Y10" s="24"/>
+      <c r="Z10" s="24"/>
+      <c r="AA10" s="24"/>
+      <c r="AB10" s="24"/>
+      <c r="AC10" s="24"/>
+      <c r="AD10" s="24"/>
+      <c r="AE10" s="24"/>
+      <c r="AF10" s="24"/>
+    </row>
+    <row r="11" spans="2:32">
       <c r="C11" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="2:10">
+      <c r="N11" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="24"/>
+      <c r="R11" s="24"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="24"/>
+      <c r="U11" s="24"/>
+      <c r="V11" s="24"/>
+      <c r="W11" s="24"/>
+      <c r="X11" s="24"/>
+      <c r="Y11" s="24"/>
+      <c r="Z11" s="24"/>
+      <c r="AA11" s="24"/>
+      <c r="AB11" s="24"/>
+      <c r="AC11" s="24"/>
+      <c r="AD11" s="24"/>
+      <c r="AE11" s="24"/>
+      <c r="AF11" s="24"/>
+    </row>
+    <row r="12" spans="2:32">
       <c r="D12" s="7" t="s">
         <v>7</v>
       </c>
@@ -1127,13 +1385,55 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="6"/>
-    </row>
-    <row r="13" spans="2:10">
+      <c r="N12" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="O12" s="24"/>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="24"/>
+      <c r="R12" s="24"/>
+      <c r="S12" s="24"/>
+      <c r="T12" s="24"/>
+      <c r="U12" s="24"/>
+      <c r="V12" s="24"/>
+      <c r="W12" s="24"/>
+      <c r="X12" s="24"/>
+      <c r="Y12" s="24"/>
+      <c r="Z12" s="24"/>
+      <c r="AA12" s="24"/>
+      <c r="AB12" s="24"/>
+      <c r="AC12" s="24"/>
+      <c r="AD12" s="24"/>
+      <c r="AE12" s="24"/>
+      <c r="AF12" s="24"/>
+    </row>
+    <row r="13" spans="2:32">
       <c r="C13" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="2:10">
+      <c r="N13" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="O13" s="24"/>
+      <c r="P13" s="24"/>
+      <c r="Q13" s="24"/>
+      <c r="R13" s="24"/>
+      <c r="S13" s="24"/>
+      <c r="T13" s="24"/>
+      <c r="U13" s="24"/>
+      <c r="V13" s="24"/>
+      <c r="W13" s="24"/>
+      <c r="X13" s="24"/>
+      <c r="Y13" s="24"/>
+      <c r="Z13" s="24"/>
+      <c r="AA13" s="24"/>
+      <c r="AB13" s="24"/>
+      <c r="AC13" s="24"/>
+      <c r="AD13" s="24"/>
+      <c r="AE13" s="24"/>
+      <c r="AF13" s="24"/>
+    </row>
+    <row r="14" spans="2:32">
       <c r="D14" s="7" t="s">
         <v>5</v>
       </c>
@@ -1143,13 +1443,55 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="6"/>
-    </row>
-    <row r="15" spans="2:10">
+      <c r="N14" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="O14" s="24"/>
+      <c r="P14" s="24"/>
+      <c r="Q14" s="24"/>
+      <c r="R14" s="24"/>
+      <c r="S14" s="24"/>
+      <c r="T14" s="24"/>
+      <c r="U14" s="24"/>
+      <c r="V14" s="24"/>
+      <c r="W14" s="24"/>
+      <c r="X14" s="24"/>
+      <c r="Y14" s="24"/>
+      <c r="Z14" s="24"/>
+      <c r="AA14" s="24"/>
+      <c r="AB14" s="24"/>
+      <c r="AC14" s="24"/>
+      <c r="AD14" s="24"/>
+      <c r="AE14" s="24"/>
+      <c r="AF14" s="24"/>
+    </row>
+    <row r="15" spans="2:32">
       <c r="C15" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="2:10">
+      <c r="N15" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="O15" s="24"/>
+      <c r="P15" s="24"/>
+      <c r="Q15" s="24"/>
+      <c r="R15" s="24"/>
+      <c r="S15" s="24"/>
+      <c r="T15" s="24"/>
+      <c r="U15" s="24"/>
+      <c r="V15" s="24"/>
+      <c r="W15" s="24"/>
+      <c r="X15" s="24"/>
+      <c r="Y15" s="24"/>
+      <c r="Z15" s="24"/>
+      <c r="AA15" s="24"/>
+      <c r="AB15" s="24"/>
+      <c r="AC15" s="24"/>
+      <c r="AD15" s="24"/>
+      <c r="AE15" s="24"/>
+      <c r="AF15" s="24"/>
+    </row>
+    <row r="16" spans="2:32">
       <c r="D16" s="7" t="s">
         <v>6</v>
       </c>
@@ -1159,13 +1501,55 @@
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="6"/>
-    </row>
-    <row r="17" spans="3:10">
+      <c r="N16" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="O16" s="24"/>
+      <c r="P16" s="24"/>
+      <c r="Q16" s="24"/>
+      <c r="R16" s="24"/>
+      <c r="S16" s="24"/>
+      <c r="T16" s="24"/>
+      <c r="U16" s="24"/>
+      <c r="V16" s="24"/>
+      <c r="W16" s="24"/>
+      <c r="X16" s="24"/>
+      <c r="Y16" s="24"/>
+      <c r="Z16" s="24"/>
+      <c r="AA16" s="24"/>
+      <c r="AB16" s="24"/>
+      <c r="AC16" s="24"/>
+      <c r="AD16" s="24"/>
+      <c r="AE16" s="24"/>
+      <c r="AF16" s="24"/>
+    </row>
+    <row r="17" spans="3:32">
       <c r="C17" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="3:10">
+      <c r="N17" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="O17" s="24"/>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="24"/>
+      <c r="R17" s="24"/>
+      <c r="S17" s="24"/>
+      <c r="T17" s="24"/>
+      <c r="U17" s="24"/>
+      <c r="V17" s="24"/>
+      <c r="W17" s="24"/>
+      <c r="X17" s="24"/>
+      <c r="Y17" s="24"/>
+      <c r="Z17" s="24"/>
+      <c r="AA17" s="24"/>
+      <c r="AB17" s="24"/>
+      <c r="AC17" s="24"/>
+      <c r="AD17" s="24"/>
+      <c r="AE17" s="24"/>
+      <c r="AF17" s="24"/>
+    </row>
+    <row r="18" spans="3:32">
       <c r="D18" s="7" t="s">
         <v>18</v>
       </c>
@@ -1177,8 +1561,27 @@
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="6"/>
-    </row>
-    <row r="19" spans="3:10">
+      <c r="N18" s="24"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="24"/>
+      <c r="Q18" s="24"/>
+      <c r="R18" s="24"/>
+      <c r="S18" s="24"/>
+      <c r="T18" s="24"/>
+      <c r="U18" s="24"/>
+      <c r="V18" s="24"/>
+      <c r="W18" s="24"/>
+      <c r="X18" s="24"/>
+      <c r="Y18" s="24"/>
+      <c r="Z18" s="24"/>
+      <c r="AA18" s="24"/>
+      <c r="AB18" s="24"/>
+      <c r="AC18" s="24"/>
+      <c r="AD18" s="24"/>
+      <c r="AE18" s="24"/>
+      <c r="AF18" s="24"/>
+    </row>
+    <row r="19" spans="3:32">
       <c r="D19" s="7" t="s">
         <v>8</v>
       </c>
@@ -1190,8 +1593,29 @@
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="6"/>
-    </row>
-    <row r="20" spans="3:10">
+      <c r="N19" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="O19" s="24"/>
+      <c r="P19" s="24"/>
+      <c r="Q19" s="24"/>
+      <c r="R19" s="24"/>
+      <c r="S19" s="24"/>
+      <c r="T19" s="24"/>
+      <c r="U19" s="24"/>
+      <c r="V19" s="24"/>
+      <c r="W19" s="24"/>
+      <c r="X19" s="24"/>
+      <c r="Y19" s="24"/>
+      <c r="Z19" s="24"/>
+      <c r="AA19" s="24"/>
+      <c r="AB19" s="24"/>
+      <c r="AC19" s="24"/>
+      <c r="AD19" s="24"/>
+      <c r="AE19" s="24"/>
+      <c r="AF19" s="24"/>
+    </row>
+    <row r="20" spans="3:32">
       <c r="D20" s="7" t="s">
         <v>9</v>
       </c>
@@ -1204,7 +1628,7 @@
       <c r="I20" s="5"/>
       <c r="J20" s="6"/>
     </row>
-    <row r="21" spans="3:10">
+    <row r="21" spans="3:32">
       <c r="D21" s="7" t="s">
         <v>10</v>
       </c>
@@ -1217,7 +1641,7 @@
       <c r="I21" s="5"/>
       <c r="J21" s="6"/>
     </row>
-    <row r="22" spans="3:10">
+    <row r="22" spans="3:32">
       <c r="D22" s="7" t="s">
         <v>23</v>
       </c>
@@ -1863,7 +2287,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3864261-7293-EB4C-A9C5-C32A1D051528}">
   <dimension ref="B2:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add Env & Library and Tool List
</commit_message>
<xml_diff>
--- a/doc/20230202_ReactApp.xlsx
+++ b/doc/20230202_ReactApp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakip/Documents/theoriacode/jisyu/20230202_ReactApp/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09B0783-6FC7-CD46-9ACD-17B63279C7CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB0DAAA2-2BE0-2F4D-8717-7BCD918FF43E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2640" yWindow="1500" windowWidth="28300" windowHeight="17440" xr2:uid="{9D86ED21-1AC9-D642-9B74-F217DA55E7A3}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>予定としている成果物</t>
     <rPh sb="0" eb="2">
@@ -451,12 +451,73 @@
   <si>
     <t>npm install --save-dev @storybook/addon-postcss tsconfig-paths-webpack-plugin @babel/plugin-proposal-class @babel/plugin-proposal-private-methods @babel/plugin-proposal-private-property-in-object tsconfig-paths-webpack-plugin @mdx-js/react</t>
   </si>
+  <si>
+    <t>npm install swr</t>
+  </si>
+  <si>
+    <t>npm install react-hook-form</t>
+  </si>
+  <si>
+    <t>環境変数</t>
+    <rPh sb="0" eb="4">
+      <t xml:space="preserve">カンキョウヘンスウ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>▼.env</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>API_BASE_URL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFD6DEEB"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>=http://localhost:8000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>NEXT_PUBLIC_API_BASE_PATH</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFD6DEEB"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>=/api/proxy</t>
+    </r>
+  </si>
+  <si>
+    <t>npm install react-content-loader</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>npm install --save-dev @types/react-content-loader</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>npm install @mui/material @mui/icons-material @emotion/react @emotion/styled</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>npm install --save-dev @testing-library/jest-dom @testing-library/react jest jest-environment-jsdom</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -491,6 +552,18 @@
       <sz val="10"/>
       <color rgb="FFF2F2F2"/>
       <name val="Monaco"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFD6DEEB"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFC792EA"/>
+      <name val="Menlo"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -748,7 +821,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1224,37 +1297,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A75F9DC-1CB6-7049-8E5D-3F652FE6EB52}">
-  <dimension ref="B2:AG43"/>
+  <dimension ref="B2:AG32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="U13" sqref="U13"/>
+    <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
   <sheetData>
-    <row r="2" spans="2:32" ht="21" thickBot="1">
+    <row r="2" spans="2:17" ht="21" thickBot="1">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="2:32">
+    <row r="3" spans="2:17">
       <c r="C3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:32">
+    <row r="4" spans="2:17">
       <c r="C4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:32" ht="21" thickBot="1">
+    <row r="6" spans="2:17" ht="21" thickBot="1">
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="2:32">
+    <row r="7" spans="2:17">
       <c r="C7" s="3" t="s">
         <v>11</v>
       </c>
@@ -1262,7 +1335,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="2:32">
+    <row r="8" spans="2:17">
       <c r="D8" s="7" t="s">
         <v>4</v>
       </c>
@@ -1278,23 +1351,8 @@
       <c r="O8" s="23"/>
       <c r="P8" s="23"/>
       <c r="Q8" s="23"/>
-      <c r="R8" s="24"/>
-      <c r="S8" s="24"/>
-      <c r="T8" s="24"/>
-      <c r="U8" s="24"/>
-      <c r="V8" s="24"/>
-      <c r="W8" s="24"/>
-      <c r="X8" s="24"/>
-      <c r="Y8" s="24"/>
-      <c r="Z8" s="24"/>
-      <c r="AA8" s="24"/>
-      <c r="AB8" s="24"/>
-      <c r="AC8" s="24"/>
-      <c r="AD8" s="24"/>
-      <c r="AE8" s="24"/>
-      <c r="AF8" s="24"/>
-    </row>
-    <row r="9" spans="2:32">
+    </row>
+    <row r="9" spans="2:17">
       <c r="C9" s="3" t="s">
         <v>15</v>
       </c>
@@ -1304,23 +1362,8 @@
       <c r="O9" s="23"/>
       <c r="P9" s="23"/>
       <c r="Q9" s="23"/>
-      <c r="R9" s="24"/>
-      <c r="S9" s="24"/>
-      <c r="T9" s="24"/>
-      <c r="U9" s="24"/>
-      <c r="V9" s="24"/>
-      <c r="W9" s="24"/>
-      <c r="X9" s="24"/>
-      <c r="Y9" s="24"/>
-      <c r="Z9" s="24"/>
-      <c r="AA9" s="24"/>
-      <c r="AB9" s="24"/>
-      <c r="AC9" s="24"/>
-      <c r="AD9" s="24"/>
-      <c r="AE9" s="24"/>
-      <c r="AF9" s="24"/>
-    </row>
-    <row r="10" spans="2:32">
+    </row>
+    <row r="10" spans="2:17">
       <c r="D10" s="7" t="s">
         <v>16</v>
       </c>
@@ -1336,23 +1379,8 @@
       <c r="O10" s="23"/>
       <c r="P10" s="23"/>
       <c r="Q10" s="23"/>
-      <c r="R10" s="24"/>
-      <c r="S10" s="24"/>
-      <c r="T10" s="24"/>
-      <c r="U10" s="24"/>
-      <c r="V10" s="24"/>
-      <c r="W10" s="24"/>
-      <c r="X10" s="24"/>
-      <c r="Y10" s="24"/>
-      <c r="Z10" s="24"/>
-      <c r="AA10" s="24"/>
-      <c r="AB10" s="24"/>
-      <c r="AC10" s="24"/>
-      <c r="AD10" s="24"/>
-      <c r="AE10" s="24"/>
-      <c r="AF10" s="24"/>
-    </row>
-    <row r="11" spans="2:32">
+    </row>
+    <row r="11" spans="2:17">
       <c r="C11" s="3" t="s">
         <v>14</v>
       </c>
@@ -1362,23 +1390,8 @@
       <c r="O11" s="23"/>
       <c r="P11" s="23"/>
       <c r="Q11" s="23"/>
-      <c r="R11" s="24"/>
-      <c r="S11" s="24"/>
-      <c r="T11" s="24"/>
-      <c r="U11" s="24"/>
-      <c r="V11" s="24"/>
-      <c r="W11" s="24"/>
-      <c r="X11" s="24"/>
-      <c r="Y11" s="24"/>
-      <c r="Z11" s="24"/>
-      <c r="AA11" s="24"/>
-      <c r="AB11" s="24"/>
-      <c r="AC11" s="24"/>
-      <c r="AD11" s="24"/>
-      <c r="AE11" s="24"/>
-      <c r="AF11" s="24"/>
-    </row>
-    <row r="12" spans="2:32">
+    </row>
+    <row r="12" spans="2:17">
       <c r="D12" s="7" t="s">
         <v>7</v>
       </c>
@@ -1394,23 +1407,8 @@
       <c r="O12" s="23"/>
       <c r="P12" s="23"/>
       <c r="Q12" s="23"/>
-      <c r="R12" s="24"/>
-      <c r="S12" s="24"/>
-      <c r="T12" s="24"/>
-      <c r="U12" s="24"/>
-      <c r="V12" s="24"/>
-      <c r="W12" s="24"/>
-      <c r="X12" s="24"/>
-      <c r="Y12" s="24"/>
-      <c r="Z12" s="24"/>
-      <c r="AA12" s="24"/>
-      <c r="AB12" s="24"/>
-      <c r="AC12" s="24"/>
-      <c r="AD12" s="24"/>
-      <c r="AE12" s="24"/>
-      <c r="AF12" s="24"/>
-    </row>
-    <row r="13" spans="2:32">
+    </row>
+    <row r="13" spans="2:17">
       <c r="C13" s="3" t="s">
         <v>12</v>
       </c>
@@ -1420,23 +1418,8 @@
       <c r="O13" s="23"/>
       <c r="P13" s="23"/>
       <c r="Q13" s="23"/>
-      <c r="R13" s="24"/>
-      <c r="S13" s="24"/>
-      <c r="T13" s="24"/>
-      <c r="U13" s="24"/>
-      <c r="V13" s="24"/>
-      <c r="W13" s="24"/>
-      <c r="X13" s="24"/>
-      <c r="Y13" s="24"/>
-      <c r="Z13" s="24"/>
-      <c r="AA13" s="24"/>
-      <c r="AB13" s="24"/>
-      <c r="AC13" s="24"/>
-      <c r="AD13" s="24"/>
-      <c r="AE13" s="24"/>
-      <c r="AF13" s="24"/>
-    </row>
-    <row r="14" spans="2:32">
+    </row>
+    <row r="14" spans="2:17">
       <c r="D14" s="7" t="s">
         <v>5</v>
       </c>
@@ -1452,23 +1435,8 @@
       <c r="O14" s="23"/>
       <c r="P14" s="23"/>
       <c r="Q14" s="23"/>
-      <c r="R14" s="24"/>
-      <c r="S14" s="24"/>
-      <c r="T14" s="24"/>
-      <c r="U14" s="24"/>
-      <c r="V14" s="24"/>
-      <c r="W14" s="24"/>
-      <c r="X14" s="24"/>
-      <c r="Y14" s="24"/>
-      <c r="Z14" s="24"/>
-      <c r="AA14" s="24"/>
-      <c r="AB14" s="24"/>
-      <c r="AC14" s="24"/>
-      <c r="AD14" s="24"/>
-      <c r="AE14" s="24"/>
-      <c r="AF14" s="24"/>
-    </row>
-    <row r="15" spans="2:32">
+    </row>
+    <row r="15" spans="2:17">
       <c r="C15" s="3" t="s">
         <v>13</v>
       </c>
@@ -1478,23 +1446,8 @@
       <c r="O15" s="23"/>
       <c r="P15" s="23"/>
       <c r="Q15" s="23"/>
-      <c r="R15" s="24"/>
-      <c r="S15" s="24"/>
-      <c r="T15" s="24"/>
-      <c r="U15" s="24"/>
-      <c r="V15" s="24"/>
-      <c r="W15" s="24"/>
-      <c r="X15" s="24"/>
-      <c r="Y15" s="24"/>
-      <c r="Z15" s="24"/>
-      <c r="AA15" s="24"/>
-      <c r="AB15" s="24"/>
-      <c r="AC15" s="24"/>
-      <c r="AD15" s="24"/>
-      <c r="AE15" s="24"/>
-      <c r="AF15" s="24"/>
-    </row>
-    <row r="16" spans="2:32">
+    </row>
+    <row r="16" spans="2:17">
       <c r="D16" s="7" t="s">
         <v>6</v>
       </c>
@@ -1510,23 +1463,8 @@
       <c r="O16" s="23"/>
       <c r="P16" s="23"/>
       <c r="Q16" s="23"/>
-      <c r="R16" s="24"/>
-      <c r="S16" s="24"/>
-      <c r="T16" s="24"/>
-      <c r="U16" s="24"/>
-      <c r="V16" s="24"/>
-      <c r="W16" s="24"/>
-      <c r="X16" s="24"/>
-      <c r="Y16" s="24"/>
-      <c r="Z16" s="24"/>
-      <c r="AA16" s="24"/>
-      <c r="AB16" s="24"/>
-      <c r="AC16" s="24"/>
-      <c r="AD16" s="24"/>
-      <c r="AE16" s="24"/>
-      <c r="AF16" s="24"/>
-    </row>
-    <row r="17" spans="3:33">
+    </row>
+    <row r="17" spans="2:33">
       <c r="C17" s="3" t="s">
         <v>17</v>
       </c>
@@ -1536,23 +1474,8 @@
       <c r="O17" s="23"/>
       <c r="P17" s="23"/>
       <c r="Q17" s="23"/>
-      <c r="R17" s="24"/>
-      <c r="S17" s="24"/>
-      <c r="T17" s="24"/>
-      <c r="U17" s="24"/>
-      <c r="V17" s="24"/>
-      <c r="W17" s="24"/>
-      <c r="X17" s="24"/>
-      <c r="Y17" s="24"/>
-      <c r="Z17" s="24"/>
-      <c r="AA17" s="24"/>
-      <c r="AB17" s="24"/>
-      <c r="AC17" s="24"/>
-      <c r="AD17" s="24"/>
-      <c r="AE17" s="24"/>
-      <c r="AF17" s="24"/>
-    </row>
-    <row r="18" spans="3:33">
+    </row>
+    <row r="18" spans="2:33">
       <c r="D18" s="7" t="s">
         <v>18</v>
       </c>
@@ -1564,27 +1487,8 @@
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="6"/>
-      <c r="N18" s="24"/>
-      <c r="O18" s="24"/>
-      <c r="P18" s="24"/>
-      <c r="Q18" s="24"/>
-      <c r="R18" s="24"/>
-      <c r="S18" s="24"/>
-      <c r="T18" s="24"/>
-      <c r="U18" s="24"/>
-      <c r="V18" s="24"/>
-      <c r="W18" s="24"/>
-      <c r="X18" s="24"/>
-      <c r="Y18" s="24"/>
-      <c r="Z18" s="24"/>
-      <c r="AA18" s="24"/>
-      <c r="AB18" s="24"/>
-      <c r="AC18" s="24"/>
-      <c r="AD18" s="24"/>
-      <c r="AE18" s="24"/>
-      <c r="AF18" s="24"/>
-    </row>
-    <row r="19" spans="3:33">
+    </row>
+    <row r="19" spans="2:33">
       <c r="D19" s="7" t="s">
         <v>8</v>
       </c>
@@ -1619,7 +1523,7 @@
       <c r="AF19" s="23"/>
       <c r="AG19" s="23"/>
     </row>
-    <row r="20" spans="3:33">
+    <row r="20" spans="2:33">
       <c r="D20" s="7" t="s">
         <v>9</v>
       </c>
@@ -1631,27 +1535,8 @@
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="6"/>
-      <c r="N20" s="24"/>
-      <c r="O20" s="24"/>
-      <c r="P20" s="24"/>
-      <c r="Q20" s="24"/>
-      <c r="R20" s="24"/>
-      <c r="S20" s="24"/>
-      <c r="T20" s="24"/>
-      <c r="U20" s="24"/>
-      <c r="V20" s="24"/>
-      <c r="W20" s="24"/>
-      <c r="X20" s="24"/>
-      <c r="Y20" s="24"/>
-      <c r="Z20" s="24"/>
-      <c r="AA20" s="24"/>
-      <c r="AB20" s="24"/>
-      <c r="AC20" s="24"/>
-      <c r="AD20" s="24"/>
-      <c r="AE20" s="24"/>
-      <c r="AF20" s="24"/>
-    </row>
-    <row r="21" spans="3:33">
+    </row>
+    <row r="21" spans="2:33">
       <c r="D21" s="7" t="s">
         <v>10</v>
       </c>
@@ -1686,7 +1571,7 @@
       <c r="AF21" s="23"/>
       <c r="AG21" s="23"/>
     </row>
-    <row r="22" spans="3:33">
+    <row r="22" spans="2:33">
       <c r="D22" s="7" t="s">
         <v>23</v>
       </c>
@@ -1698,466 +1583,119 @@
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="6"/>
-      <c r="N22" s="24"/>
-      <c r="O22" s="24"/>
-      <c r="P22" s="24"/>
-      <c r="Q22" s="24"/>
-      <c r="R22" s="24"/>
-      <c r="S22" s="24"/>
-      <c r="T22" s="24"/>
-      <c r="U22" s="24"/>
-      <c r="V22" s="24"/>
-      <c r="W22" s="24"/>
-      <c r="X22" s="24"/>
-      <c r="Y22" s="24"/>
-      <c r="Z22" s="24"/>
-      <c r="AA22" s="24"/>
-      <c r="AB22" s="24"/>
-      <c r="AC22" s="24"/>
-      <c r="AD22" s="24"/>
-      <c r="AE22" s="24"/>
-      <c r="AF22" s="24"/>
-    </row>
-    <row r="23" spans="3:33">
-      <c r="N23" s="24"/>
-      <c r="O23" s="24"/>
-      <c r="P23" s="24"/>
-      <c r="Q23" s="24"/>
-      <c r="R23" s="24"/>
-      <c r="S23" s="24"/>
-      <c r="T23" s="24"/>
-      <c r="U23" s="24"/>
-      <c r="V23" s="24"/>
-      <c r="W23" s="24"/>
-      <c r="X23" s="24"/>
-      <c r="Y23" s="24"/>
-      <c r="Z23" s="24"/>
-      <c r="AA23" s="24"/>
-      <c r="AB23" s="24"/>
-      <c r="AC23" s="24"/>
-      <c r="AD23" s="24"/>
-      <c r="AE23" s="24"/>
-      <c r="AF23" s="24"/>
-    </row>
-    <row r="24" spans="3:33">
-      <c r="N24" s="24"/>
-      <c r="O24" s="24"/>
-      <c r="P24" s="24"/>
-      <c r="Q24" s="24"/>
-      <c r="R24" s="24"/>
-      <c r="S24" s="24"/>
-      <c r="T24" s="24"/>
-      <c r="U24" s="24"/>
-      <c r="V24" s="24"/>
-      <c r="W24" s="24"/>
-      <c r="X24" s="24"/>
-      <c r="Y24" s="24"/>
-      <c r="Z24" s="24"/>
-      <c r="AA24" s="24"/>
-      <c r="AB24" s="24"/>
-      <c r="AC24" s="24"/>
-      <c r="AD24" s="24"/>
-      <c r="AE24" s="24"/>
-      <c r="AF24" s="24"/>
-    </row>
-    <row r="25" spans="3:33">
-      <c r="N25" s="24"/>
-      <c r="O25" s="24"/>
-      <c r="P25" s="24"/>
-      <c r="Q25" s="24"/>
-      <c r="R25" s="24"/>
-      <c r="S25" s="24"/>
-      <c r="T25" s="24"/>
-      <c r="U25" s="24"/>
-      <c r="V25" s="24"/>
-      <c r="W25" s="24"/>
-      <c r="X25" s="24"/>
-      <c r="Y25" s="24"/>
-      <c r="Z25" s="24"/>
-      <c r="AA25" s="24"/>
-      <c r="AB25" s="24"/>
-      <c r="AC25" s="24"/>
-      <c r="AD25" s="24"/>
-      <c r="AE25" s="24"/>
-      <c r="AF25" s="24"/>
-    </row>
-    <row r="26" spans="3:33">
-      <c r="N26" s="24"/>
-      <c r="O26" s="24"/>
-      <c r="P26" s="24"/>
-      <c r="Q26" s="24"/>
-      <c r="R26" s="24"/>
-      <c r="S26" s="24"/>
-      <c r="T26" s="24"/>
-      <c r="U26" s="24"/>
-      <c r="V26" s="24"/>
-      <c r="W26" s="24"/>
-      <c r="X26" s="24"/>
-      <c r="Y26" s="24"/>
-      <c r="Z26" s="24"/>
-      <c r="AA26" s="24"/>
-      <c r="AB26" s="24"/>
-      <c r="AC26" s="24"/>
-      <c r="AD26" s="24"/>
-      <c r="AE26" s="24"/>
-      <c r="AF26" s="24"/>
-    </row>
-    <row r="27" spans="3:33">
-      <c r="N27" s="24"/>
-      <c r="O27" s="24"/>
-      <c r="P27" s="24"/>
-      <c r="Q27" s="24"/>
-      <c r="R27" s="24"/>
-      <c r="S27" s="24"/>
-      <c r="T27" s="24"/>
-      <c r="U27" s="24"/>
-      <c r="V27" s="24"/>
-      <c r="W27" s="24"/>
-      <c r="X27" s="24"/>
-      <c r="Y27" s="24"/>
-      <c r="Z27" s="24"/>
-      <c r="AA27" s="24"/>
-      <c r="AB27" s="24"/>
-      <c r="AC27" s="24"/>
-      <c r="AD27" s="24"/>
-      <c r="AE27" s="24"/>
-      <c r="AF27" s="24"/>
-    </row>
-    <row r="28" spans="3:33">
-      <c r="N28" s="24"/>
-      <c r="O28" s="24"/>
-      <c r="P28" s="24"/>
-      <c r="Q28" s="24"/>
-      <c r="R28" s="24"/>
-      <c r="S28" s="24"/>
-      <c r="T28" s="24"/>
-      <c r="U28" s="24"/>
-      <c r="V28" s="24"/>
-      <c r="W28" s="24"/>
-      <c r="X28" s="24"/>
-      <c r="Y28" s="24"/>
-      <c r="Z28" s="24"/>
-      <c r="AA28" s="24"/>
-      <c r="AB28" s="24"/>
-      <c r="AC28" s="24"/>
-      <c r="AD28" s="24"/>
-      <c r="AE28" s="24"/>
-      <c r="AF28" s="24"/>
-    </row>
-    <row r="29" spans="3:33">
-      <c r="N29" s="24"/>
-      <c r="O29" s="24"/>
-      <c r="P29" s="24"/>
-      <c r="Q29" s="24"/>
-      <c r="R29" s="24"/>
-      <c r="S29" s="24"/>
-      <c r="T29" s="24"/>
-      <c r="U29" s="24"/>
-      <c r="V29" s="24"/>
-      <c r="W29" s="24"/>
-      <c r="X29" s="24"/>
-      <c r="Y29" s="24"/>
-      <c r="Z29" s="24"/>
-      <c r="AA29" s="24"/>
-      <c r="AB29" s="24"/>
-      <c r="AC29" s="24"/>
-      <c r="AD29" s="24"/>
-      <c r="AE29" s="24"/>
-      <c r="AF29" s="24"/>
-    </row>
-    <row r="30" spans="3:33">
-      <c r="N30" s="24"/>
-      <c r="O30" s="24"/>
-      <c r="P30" s="24"/>
-      <c r="Q30" s="24"/>
-      <c r="R30" s="24"/>
-      <c r="S30" s="24"/>
-      <c r="T30" s="24"/>
-      <c r="U30" s="24"/>
-      <c r="V30" s="24"/>
-      <c r="W30" s="24"/>
-      <c r="X30" s="24"/>
-      <c r="Y30" s="24"/>
-      <c r="Z30" s="24"/>
-      <c r="AA30" s="24"/>
-      <c r="AB30" s="24"/>
-      <c r="AC30" s="24"/>
-      <c r="AD30" s="24"/>
-      <c r="AE30" s="24"/>
-      <c r="AF30" s="24"/>
-    </row>
-    <row r="31" spans="3:33">
-      <c r="N31" s="24"/>
-      <c r="O31" s="24"/>
-      <c r="P31" s="24"/>
-      <c r="Q31" s="24"/>
-      <c r="R31" s="24"/>
-      <c r="S31" s="24"/>
-      <c r="T31" s="24"/>
-      <c r="U31" s="24"/>
-      <c r="V31" s="24"/>
-      <c r="W31" s="24"/>
-      <c r="X31" s="24"/>
-      <c r="Y31" s="24"/>
-      <c r="Z31" s="24"/>
-      <c r="AA31" s="24"/>
-      <c r="AB31" s="24"/>
-      <c r="AC31" s="24"/>
-      <c r="AD31" s="24"/>
-      <c r="AE31" s="24"/>
-      <c r="AF31" s="24"/>
-    </row>
-    <row r="32" spans="3:33">
-      <c r="N32" s="24"/>
-      <c r="O32" s="24"/>
-      <c r="P32" s="24"/>
-      <c r="Q32" s="24"/>
-      <c r="R32" s="24"/>
-      <c r="S32" s="24"/>
-      <c r="T32" s="24"/>
-      <c r="U32" s="24"/>
-      <c r="V32" s="24"/>
-      <c r="W32" s="24"/>
-      <c r="X32" s="24"/>
-      <c r="Y32" s="24"/>
-      <c r="Z32" s="24"/>
-      <c r="AA32" s="24"/>
-      <c r="AB32" s="24"/>
-      <c r="AC32" s="24"/>
-      <c r="AD32" s="24"/>
-      <c r="AE32" s="24"/>
-      <c r="AF32" s="24"/>
-    </row>
-    <row r="33" spans="14:32">
-      <c r="N33" s="24"/>
-      <c r="O33" s="24"/>
-      <c r="P33" s="24"/>
-      <c r="Q33" s="24"/>
-      <c r="R33" s="24"/>
-      <c r="S33" s="24"/>
-      <c r="T33" s="24"/>
-      <c r="U33" s="24"/>
-      <c r="V33" s="24"/>
-      <c r="W33" s="24"/>
-      <c r="X33" s="24"/>
-      <c r="Y33" s="24"/>
-      <c r="Z33" s="24"/>
-      <c r="AA33" s="24"/>
-      <c r="AB33" s="24"/>
-      <c r="AC33" s="24"/>
-      <c r="AD33" s="24"/>
-      <c r="AE33" s="24"/>
-      <c r="AF33" s="24"/>
-    </row>
-    <row r="34" spans="14:32">
-      <c r="N34" s="24"/>
-      <c r="O34" s="24"/>
-      <c r="P34" s="24"/>
-      <c r="Q34" s="24"/>
-      <c r="R34" s="24"/>
-      <c r="S34" s="24"/>
-      <c r="T34" s="24"/>
-      <c r="U34" s="24"/>
-      <c r="V34" s="24"/>
-      <c r="W34" s="24"/>
-      <c r="X34" s="24"/>
-      <c r="Y34" s="24"/>
-      <c r="Z34" s="24"/>
-      <c r="AA34" s="24"/>
-      <c r="AB34" s="24"/>
-      <c r="AC34" s="24"/>
-      <c r="AD34" s="24"/>
-      <c r="AE34" s="24"/>
-      <c r="AF34" s="24"/>
-    </row>
-    <row r="35" spans="14:32">
-      <c r="N35" s="24"/>
-      <c r="O35" s="24"/>
-      <c r="P35" s="24"/>
-      <c r="Q35" s="24"/>
-      <c r="R35" s="24"/>
-      <c r="S35" s="24"/>
-      <c r="T35" s="24"/>
-      <c r="U35" s="24"/>
-      <c r="V35" s="24"/>
-      <c r="W35" s="24"/>
-      <c r="X35" s="24"/>
-      <c r="Y35" s="24"/>
-      <c r="Z35" s="24"/>
-      <c r="AA35" s="24"/>
-      <c r="AB35" s="24"/>
-      <c r="AC35" s="24"/>
-      <c r="AD35" s="24"/>
-      <c r="AE35" s="24"/>
-      <c r="AF35" s="24"/>
-    </row>
-    <row r="36" spans="14:32">
-      <c r="N36" s="24"/>
-      <c r="O36" s="24"/>
-      <c r="P36" s="24"/>
-      <c r="Q36" s="24"/>
-      <c r="R36" s="24"/>
-      <c r="S36" s="24"/>
-      <c r="T36" s="24"/>
-      <c r="U36" s="24"/>
-      <c r="V36" s="24"/>
-      <c r="W36" s="24"/>
-      <c r="X36" s="24"/>
-      <c r="Y36" s="24"/>
-      <c r="Z36" s="24"/>
-      <c r="AA36" s="24"/>
-      <c r="AB36" s="24"/>
-      <c r="AC36" s="24"/>
-      <c r="AD36" s="24"/>
-      <c r="AE36" s="24"/>
-      <c r="AF36" s="24"/>
-    </row>
-    <row r="37" spans="14:32">
-      <c r="N37" s="24"/>
-      <c r="O37" s="24"/>
-      <c r="P37" s="24"/>
-      <c r="Q37" s="24"/>
-      <c r="R37" s="24"/>
-      <c r="S37" s="24"/>
-      <c r="T37" s="24"/>
-      <c r="U37" s="24"/>
-      <c r="V37" s="24"/>
-      <c r="W37" s="24"/>
-      <c r="X37" s="24"/>
-      <c r="Y37" s="24"/>
-      <c r="Z37" s="24"/>
-      <c r="AA37" s="24"/>
-      <c r="AB37" s="24"/>
-      <c r="AC37" s="24"/>
-      <c r="AD37" s="24"/>
-      <c r="AE37" s="24"/>
-      <c r="AF37" s="24"/>
-    </row>
-    <row r="38" spans="14:32">
-      <c r="N38" s="24"/>
-      <c r="O38" s="24"/>
-      <c r="P38" s="24"/>
-      <c r="Q38" s="24"/>
-      <c r="R38" s="24"/>
-      <c r="S38" s="24"/>
-      <c r="T38" s="24"/>
-      <c r="U38" s="24"/>
-      <c r="V38" s="24"/>
-      <c r="W38" s="24"/>
-      <c r="X38" s="24"/>
-      <c r="Y38" s="24"/>
-      <c r="Z38" s="24"/>
-      <c r="AA38" s="24"/>
-      <c r="AB38" s="24"/>
-      <c r="AC38" s="24"/>
-      <c r="AD38" s="24"/>
-      <c r="AE38" s="24"/>
-      <c r="AF38" s="24"/>
-    </row>
-    <row r="39" spans="14:32">
-      <c r="N39" s="24"/>
-      <c r="O39" s="24"/>
-      <c r="P39" s="24"/>
-      <c r="Q39" s="24"/>
-      <c r="R39" s="24"/>
-      <c r="S39" s="24"/>
-      <c r="T39" s="24"/>
-      <c r="U39" s="24"/>
-      <c r="V39" s="24"/>
-      <c r="W39" s="24"/>
-      <c r="X39" s="24"/>
-      <c r="Y39" s="24"/>
-      <c r="Z39" s="24"/>
-      <c r="AA39" s="24"/>
-      <c r="AB39" s="24"/>
-      <c r="AC39" s="24"/>
-      <c r="AD39" s="24"/>
-      <c r="AE39" s="24"/>
-      <c r="AF39" s="24"/>
-    </row>
-    <row r="40" spans="14:32">
-      <c r="N40" s="24"/>
-      <c r="O40" s="24"/>
-      <c r="P40" s="24"/>
-      <c r="Q40" s="24"/>
-      <c r="R40" s="24"/>
-      <c r="S40" s="24"/>
-      <c r="T40" s="24"/>
-      <c r="U40" s="24"/>
-      <c r="V40" s="24"/>
-      <c r="W40" s="24"/>
-      <c r="X40" s="24"/>
-      <c r="Y40" s="24"/>
-      <c r="Z40" s="24"/>
-      <c r="AA40" s="24"/>
-      <c r="AB40" s="24"/>
-      <c r="AC40" s="24"/>
-      <c r="AD40" s="24"/>
-      <c r="AE40" s="24"/>
-      <c r="AF40" s="24"/>
-    </row>
-    <row r="41" spans="14:32">
-      <c r="N41" s="24"/>
-      <c r="O41" s="24"/>
-      <c r="P41" s="24"/>
-      <c r="Q41" s="24"/>
-      <c r="R41" s="24"/>
-      <c r="S41" s="24"/>
-      <c r="T41" s="24"/>
-      <c r="U41" s="24"/>
-      <c r="V41" s="24"/>
-      <c r="W41" s="24"/>
-      <c r="X41" s="24"/>
-      <c r="Y41" s="24"/>
-      <c r="Z41" s="24"/>
-      <c r="AA41" s="24"/>
-      <c r="AB41" s="24"/>
-      <c r="AC41" s="24"/>
-      <c r="AD41" s="24"/>
-      <c r="AE41" s="24"/>
-      <c r="AF41" s="24"/>
-    </row>
-    <row r="42" spans="14:32">
-      <c r="N42" s="24"/>
-      <c r="O42" s="24"/>
-      <c r="P42" s="24"/>
-      <c r="Q42" s="24"/>
-      <c r="R42" s="24"/>
-      <c r="S42" s="24"/>
-      <c r="T42" s="24"/>
-      <c r="U42" s="24"/>
-      <c r="V42" s="24"/>
-      <c r="W42" s="24"/>
-      <c r="X42" s="24"/>
-      <c r="Y42" s="24"/>
-      <c r="Z42" s="24"/>
-      <c r="AA42" s="24"/>
-      <c r="AB42" s="24"/>
-      <c r="AC42" s="24"/>
-      <c r="AD42" s="24"/>
-      <c r="AE42" s="24"/>
-      <c r="AF42" s="24"/>
-    </row>
-    <row r="43" spans="14:32">
-      <c r="N43" s="24"/>
-      <c r="O43" s="24"/>
-      <c r="P43" s="24"/>
-      <c r="Q43" s="24"/>
-      <c r="R43" s="24"/>
-      <c r="S43" s="24"/>
-      <c r="T43" s="24"/>
-      <c r="U43" s="24"/>
-      <c r="V43" s="24"/>
-      <c r="W43" s="24"/>
-      <c r="X43" s="24"/>
-      <c r="Y43" s="24"/>
-      <c r="Z43" s="24"/>
-      <c r="AA43" s="24"/>
-      <c r="AB43" s="24"/>
-      <c r="AC43" s="24"/>
-      <c r="AD43" s="24"/>
-      <c r="AE43" s="24"/>
-      <c r="AF43" s="24"/>
+    </row>
+    <row r="23" spans="2:33">
+      <c r="N23" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="O23" s="23"/>
+      <c r="P23" s="23"/>
+      <c r="Q23" s="23"/>
+      <c r="R23" s="23"/>
+      <c r="S23" s="23"/>
+      <c r="T23" s="23"/>
+      <c r="U23" s="23"/>
+      <c r="V23" s="23"/>
+      <c r="W23" s="23"/>
+    </row>
+    <row r="24" spans="2:33" ht="21" thickBot="1">
+      <c r="B24" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="2:33">
+      <c r="C25" t="s">
+        <v>60</v>
+      </c>
+      <c r="N25" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="O25" s="23"/>
+      <c r="P25" s="23"/>
+      <c r="Q25" s="23"/>
+      <c r="R25" s="23"/>
+      <c r="S25" s="23"/>
+      <c r="T25" s="23"/>
+      <c r="U25" s="23"/>
+      <c r="V25" s="23"/>
+      <c r="W25" s="23"/>
+    </row>
+    <row r="26" spans="2:33">
+      <c r="D26" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="23"/>
+    </row>
+    <row r="27" spans="2:33">
+      <c r="D27" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
+      <c r="N27" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="O27" s="23"/>
+      <c r="P27" s="23"/>
+      <c r="Q27" s="23"/>
+      <c r="R27" s="23"/>
+      <c r="S27" s="23"/>
+      <c r="T27" s="23"/>
+      <c r="U27" s="23"/>
+      <c r="V27" s="23"/>
+      <c r="W27" s="23"/>
+    </row>
+    <row r="28" spans="2:33">
+      <c r="N28" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="O28" s="23"/>
+      <c r="P28" s="23"/>
+      <c r="Q28" s="23"/>
+      <c r="R28" s="23"/>
+      <c r="S28" s="23"/>
+      <c r="T28" s="23"/>
+      <c r="U28" s="23"/>
+      <c r="V28" s="23"/>
+      <c r="W28" s="23"/>
+    </row>
+    <row r="30" spans="2:33">
+      <c r="N30" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="O30" s="23"/>
+      <c r="P30" s="23"/>
+      <c r="Q30" s="23"/>
+      <c r="R30" s="23"/>
+      <c r="S30" s="23"/>
+      <c r="T30" s="23"/>
+      <c r="U30" s="23"/>
+      <c r="V30" s="23"/>
+      <c r="W30" s="23"/>
+    </row>
+    <row r="32" spans="2:33">
+      <c r="N32" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="O32" s="23"/>
+      <c r="P32" s="23"/>
+      <c r="Q32" s="23"/>
+      <c r="R32" s="23"/>
+      <c r="S32" s="23"/>
+      <c r="T32" s="23"/>
+      <c r="U32" s="23"/>
+      <c r="V32" s="23"/>
+      <c r="W32" s="23"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>